<commit_message>
prepared all front for facts functionalty. Missing back of front-end
</commit_message>
<xml_diff>
--- a/assets/Countries-Continents-csv.xlsx
+++ b/assets/Countries-Continents-csv.xlsx
@@ -20,7 +20,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Countries-Continents-csv'!$A$1:$D$195</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -2589,37 +2589,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="24">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="21">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -3129,8 +3099,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D195"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A184" sqref="A184:D195"/>
+    <sheetView topLeftCell="A96" workbookViewId="0">
+      <selection activeCell="B117" sqref="B117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5873,14 +5843,14 @@
   </sheetData>
   <autoFilter ref="A1:D195"/>
   <conditionalFormatting sqref="D14">
-    <cfRule type="duplicateValues" dxfId="23" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="20" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="duplicateValues" dxfId="22" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="19" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="duplicateValues" dxfId="21" priority="1"/>
-    <cfRule type="duplicateValues" dxfId="20" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="18" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="17" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -10364,8 +10334,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="A61" sqref="A61"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11795,10 +11765,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D13">
-    <cfRule type="duplicateValues" dxfId="19" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="16" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D54">
-    <cfRule type="duplicateValues" dxfId="18" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="15" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -12975,11 +12945,11 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1:D44">
-    <cfRule type="duplicateValues" dxfId="17" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="14" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C44">
-    <cfRule type="duplicateValues" dxfId="16" priority="1"/>
-    <cfRule type="duplicateValues" dxfId="15" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="13" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="12" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -12989,7 +12959,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G53"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="A53" sqref="A53"/>
     </sheetView>
   </sheetViews>
@@ -14234,11 +14204,11 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1:D47">
-    <cfRule type="duplicateValues" dxfId="14" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="11" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C47">
-    <cfRule type="duplicateValues" dxfId="13" priority="1"/>
-    <cfRule type="duplicateValues" dxfId="12" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -14320,7 +14290,7 @@
         <v>244</v>
       </c>
       <c r="E3" t="str">
-        <f t="shared" ref="E3:E23" si="0">CONCATENATE(E2,",","'",C3,"'")</f>
+        <f t="shared" ref="E3:E22" si="0">CONCATENATE(E2,",","'",C3,"'")</f>
         <v>'Antigua and Barbuda','Bahamas','Barbados'</v>
       </c>
       <c r="F3" t="str">
@@ -14869,11 +14839,11 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1:D23">
-    <cfRule type="duplicateValues" dxfId="11" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C23">
-    <cfRule type="duplicateValues" dxfId="10" priority="1"/>
-    <cfRule type="duplicateValues" dxfId="9" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -15221,8 +15191,8 @@
     <cfRule type="duplicateValues" dxfId="5" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C12">
-    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
-    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -15619,11 +15589,11 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1:D14">
-    <cfRule type="duplicateValues" dxfId="8" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C14">
-    <cfRule type="duplicateValues" dxfId="7" priority="1"/>
-    <cfRule type="duplicateValues" dxfId="6" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>